<commit_message>
testing orienation of stms in excel file
</commit_message>
<xml_diff>
--- a/calc/ozone STM calc setup v00b.xlsx
+++ b/calc/ozone STM calc setup v00b.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CalcDir\TRACI_ozone_stm\calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6835BA76-BC93-4927-98D2-37E1F7A3D8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257246D2-8A47-4CE6-9B31-4A7B2B0E5365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{BD39A979-CEB5-421F-A893-2A15417D7C3E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{BD39A979-CEB5-421F-A893-2A15417D7C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="2" r:id="rId1"/>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="280">
   <si>
     <t>File unique name</t>
   </si>
@@ -1124,7 +1124,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -1161,6 +1161,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1457,8 +1460,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DF60613B-B2E8-48B2-AE4F-B39C7018B202}" name="Tbl.SpatialTransforms" displayName="Tbl.SpatialTransforms" ref="B10:N14" totalsRowShown="0">
-  <autoFilter ref="B10:N14" xr:uid="{DF60613B-B2E8-48B2-AE4F-B39C7018B202}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DF60613B-B2E8-48B2-AE4F-B39C7018B202}" name="Tbl.SpatialTransforms" displayName="Tbl.SpatialTransforms" ref="B10:N20" totalsRowShown="0">
+  <autoFilter ref="B10:N20" xr:uid="{DF60613B-B2E8-48B2-AE4F-B39C7018B202}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{87286839-84B9-43B8-B3CC-7A5ACD26A242}" name="STM unique name">
       <calculatedColumnFormula>Tbl.SpatialTransforms[[#This Row],[File name]]</calculatedColumnFormula>
@@ -1477,7 +1480,7 @@
     <tableColumn id="6" xr3:uid="{0517F68E-B086-4B29-BCBB-FD080B95A1FD}" name="Weight Data"/>
     <tableColumn id="13" xr3:uid="{941AE024-63C8-477F-9C19-AB394C4E3067}" name="Use Existing"/>
     <tableColumn id="7" xr3:uid="{DC381ACA-0C61-4D84-BCD2-331C1153758A}" name="Auto file name" dataDxfId="2">
-      <calculatedColumnFormula>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</calculatedColumnFormula>
+      <calculatedColumnFormula>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_Wt-"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TblStyle_Med2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1971,8 +1974,8 @@
         <v>air_FF_NOx</v>
       </c>
       <c r="O8" t="str" cm="1">
-        <f t="array" ref="O8:O11">Tbl.SpatialTransforms[STM unique name]</f>
-        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Pop2010</v>
+        <f t="array" ref="O8:O17">Tbl.SpatialTransforms[STM unique name]</f>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Wt-Pop2010</v>
       </c>
       <c r="Q8" t="str" cm="1">
         <f t="array" ref="Q8:Q16">Tbl.Flows[Flow unique Name]</f>
@@ -2034,7 +2037,7 @@
         <v>air_FF_NHx</v>
       </c>
       <c r="O9" t="str">
-        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010</v>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Wt-Pop2010</v>
       </c>
       <c r="Q9" t="str">
         <v>NO</v>
@@ -2075,7 +2078,7 @@
         <v>air_FF_SOx</v>
       </c>
       <c r="O10" t="str">
-        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_urb_New-Countries_Pop2010</v>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_urb_New-Countries_Wt-Pop2010</v>
       </c>
       <c r="Q10" t="str">
         <v>NO2</v>
@@ -2113,7 +2116,7 @@
         <v>ecoreg_EFs</v>
       </c>
       <c r="O11" t="str">
-        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_urb_New-Countries_Pop2010</v>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_urb_New-Countries_Wt-Pop2010</v>
       </c>
       <c r="Q11" t="str">
         <v>NHx</v>
@@ -2135,6 +2138,9 @@
       <c r="N12" t="str">
         <v>ecoreg_GEPs</v>
       </c>
+      <c r="O12" t="str">
+        <v>STM3_newReceive_Orig-ArchFullUrb2v01_prep01_New-Countries_Wt-Pop2010</v>
+      </c>
       <c r="Q12" t="str">
         <v>NH3</v>
       </c>
@@ -2155,6 +2161,9 @@
       <c r="N13" t="str">
         <v>soil_RFs_NH4</v>
       </c>
+      <c r="O13" t="str">
+        <v>STM3_newReceive_Orig-ArchFullUrb2v01_prep01_urb_New-Countries_Wt-Pop2010</v>
+      </c>
       <c r="Q13" t="str">
         <v>NH4</v>
       </c>
@@ -2178,6 +2187,9 @@
       <c r="N14" t="str">
         <v>soil_RFs_NO3</v>
       </c>
+      <c r="O14" t="str">
+        <v>STM3_newReceive_Orig-Countries_New-ArchFullUrb2v01_prep01_Wt-Pop2010</v>
+      </c>
       <c r="Q14" t="str">
         <v>SOx</v>
       </c>
@@ -2195,6 +2207,9 @@
       <c r="N15" t="str">
         <v>soil_RFs_SOx</v>
       </c>
+      <c r="O15" t="str">
+        <v>STM3_newReceive_Orig-Countries_New-ArchFullUrb2v01_prep01_urb_Wt-Pop2010</v>
+      </c>
       <c r="Q15" t="str">
         <v>SO2</v>
       </c>
@@ -2212,6 +2227,9 @@
       <c r="N16" t="str">
         <v>AnthroVOCs_v01_gpkg</v>
       </c>
+      <c r="O16" t="str">
+        <v>STM3_newEmit_Orig-Countries_New-ArchFullUrb2v01_prep01_Wt-Pop2010</v>
+      </c>
       <c r="Q16" t="str">
         <v>SO</v>
       </c>
@@ -2228,6 +2246,9 @@
       </c>
       <c r="N17" t="str">
         <v>AnthroVOCs_v01_tif</v>
+      </c>
+      <c r="O17" t="str">
+        <v>STM3_newEmit_Orig-Countries_New-ArchFullUrb2v01_prep01_urb_Wt-Pop2010</v>
       </c>
       <c r="V17" t="str">
         <v>Edgar Air Gen NH3</v>
@@ -2462,7 +2483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2502FB-B45F-43BB-8645-D93E9F9C6CDF}">
   <dimension ref="B2:O147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -6008,10 +6029,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD1D767F-008E-40CD-A786-127BCF11776D}">
-  <dimension ref="B4:N14"/>
+  <dimension ref="B4:N20"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6032,8 +6053,8 @@
         <v>137</v>
       </c>
       <c r="C4" t="str" cm="1">
-        <f t="array" ref="C4">_xlfn.TEXTJOIN(", ",TRUE, "'"&amp;B11:B14&amp;"'")</f>
-        <v>'STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Pop2010', 'STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010', 'STM3_newEmit_Orig-ArchFullUrb2v01_prep01_urb_New-Countries_Pop2010', 'STM3_newEmit_Orig-ArchFullUrb2v02_prep01_urb_New-Countries_Pop2010'</v>
+        <f t="array" ref="C4">_xlfn.TEXTJOIN(", ",TRUE, "'"&amp;B11:B20&amp;"'")</f>
+        <v>'STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Wt-Pop2010', 'STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Wt-Pop2010', 'STM3_newEmit_Orig-ArchFullUrb2v01_prep01_urb_New-Countries_Wt-Pop2010', 'STM3_newEmit_Orig-ArchFullUrb2v02_prep01_urb_New-Countries_Wt-Pop2010', 'STM3_newReceive_Orig-ArchFullUrb2v01_prep01_New-Countries_Wt-Pop2010', 'STM3_newReceive_Orig-ArchFullUrb2v01_prep01_urb_New-Countries_Wt-Pop2010', 'STM3_newReceive_Orig-Countries_New-ArchFullUrb2v01_prep01_Wt-Pop2010', 'STM3_newReceive_Orig-Countries_New-ArchFullUrb2v01_prep01_urb_Wt-Pop2010', 'STM3_newEmit_Orig-Countries_New-ArchFullUrb2v01_prep01_Wt-Pop2010', 'STM3_newEmit_Orig-Countries_New-ArchFullUrb2v01_prep01_urb_Wt-Pop2010'</v>
       </c>
     </row>
     <row r="6" spans="2:14">
@@ -6099,14 +6120,14 @@
     <row r="11" spans="2:14">
       <c r="B11" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
-        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Pop2010</v>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Wt-Pop2010</v>
       </c>
       <c r="D11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
-        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Pop2010</v>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Wt-Pop2010</v>
       </c>
       <c r="H11" t="s">
         <v>194</v>
@@ -6127,21 +6148,21 @@
         <v>1</v>
       </c>
       <c r="N11" t="str">
-        <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
-        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Pop2010</v>
+        <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_Wt-"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Wt-Pop2010</v>
       </c>
     </row>
     <row r="12" spans="2:14">
       <c r="B12" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
-        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010</v>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Wt-Pop2010</v>
       </c>
       <c r="D12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
-        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010</v>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Wt-Pop2010</v>
       </c>
       <c r="H12" t="s">
         <v>194</v>
@@ -6162,21 +6183,21 @@
         <v>1</v>
       </c>
       <c r="N12" t="str">
-        <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
-        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010</v>
+        <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_Wt-"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Wt-Pop2010</v>
       </c>
     </row>
     <row r="13" spans="2:14">
       <c r="B13" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
-        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_urb_New-Countries_Pop2010</v>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_urb_New-Countries_Wt-Pop2010</v>
       </c>
       <c r="D13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
-        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_urb_New-Countries_Pop2010</v>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_urb_New-Countries_Wt-Pop2010</v>
       </c>
       <c r="H13" t="s">
         <v>194</v>
@@ -6197,21 +6218,21 @@
         <v>1</v>
       </c>
       <c r="N13" t="str">
-        <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
-        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_urb_New-Countries_Pop2010</v>
+        <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_Wt-"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_urb_New-Countries_Wt-Pop2010</v>
       </c>
     </row>
     <row r="14" spans="2:14">
       <c r="B14" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
-        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_urb_New-Countries_Pop2010</v>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_urb_New-Countries_Wt-Pop2010</v>
       </c>
       <c r="D14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
-        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_urb_New-Countries_Pop2010</v>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_urb_New-Countries_Wt-Pop2010</v>
       </c>
       <c r="H14" t="s">
         <v>194</v>
@@ -6232,23 +6253,233 @@
         <v>1</v>
       </c>
       <c r="N14" t="str">
-        <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
-        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_urb_New-Countries_Pop2010</v>
+        <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_Wt-"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_urb_New-Countries_Wt-Pop2010</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14">
+      <c r="B15" t="str">
+        <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
+        <v>STM3_newReceive_Orig-ArchFullUrb2v01_prep01_New-Countries_Wt-Pop2010</v>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" t="str">
+        <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
+        <v>STM3_newReceive_Orig-ArchFullUrb2v01_prep01_New-Countries_Wt-Pop2010</v>
+      </c>
+      <c r="H15" t="s">
+        <v>194</v>
+      </c>
+      <c r="I15" t="s">
+        <v>116</v>
+      </c>
+      <c r="J15" t="s">
+        <v>272</v>
+      </c>
+      <c r="K15" t="s">
+        <v>28</v>
+      </c>
+      <c r="L15" t="s">
+        <v>32</v>
+      </c>
+      <c r="M15" t="b">
+        <v>1</v>
+      </c>
+      <c r="N15" s="14" t="str">
+        <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_Wt-"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
+        <v>STM3_newReceive_Orig-ArchFullUrb2v01_prep01_New-Countries_Wt-Pop2010</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14">
+      <c r="B16" t="str">
+        <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
+        <v>STM3_newReceive_Orig-ArchFullUrb2v01_prep01_urb_New-Countries_Wt-Pop2010</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" t="str">
+        <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
+        <v>STM3_newReceive_Orig-ArchFullUrb2v01_prep01_urb_New-Countries_Wt-Pop2010</v>
+      </c>
+      <c r="H16" t="s">
+        <v>194</v>
+      </c>
+      <c r="I16" t="s">
+        <v>116</v>
+      </c>
+      <c r="J16" t="s">
+        <v>274</v>
+      </c>
+      <c r="K16" t="s">
+        <v>28</v>
+      </c>
+      <c r="L16" t="s">
+        <v>32</v>
+      </c>
+      <c r="M16" t="b">
+        <v>1</v>
+      </c>
+      <c r="N16" s="14" t="str">
+        <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_Wt-"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
+        <v>STM3_newReceive_Orig-ArchFullUrb2v01_prep01_urb_New-Countries_Wt-Pop2010</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14">
+      <c r="B17" t="str">
+        <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
+        <v>STM3_newReceive_Orig-Countries_New-ArchFullUrb2v01_prep01_Wt-Pop2010</v>
+      </c>
+      <c r="D17" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" t="str">
+        <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
+        <v>STM3_newReceive_Orig-Countries_New-ArchFullUrb2v01_prep01_Wt-Pop2010</v>
+      </c>
+      <c r="H17" t="s">
+        <v>194</v>
+      </c>
+      <c r="I17" t="s">
+        <v>116</v>
+      </c>
+      <c r="J17" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" t="s">
+        <v>272</v>
+      </c>
+      <c r="L17" t="s">
+        <v>32</v>
+      </c>
+      <c r="M17" t="b">
+        <v>1</v>
+      </c>
+      <c r="N17" s="14" t="str">
+        <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_Wt-"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
+        <v>STM3_newReceive_Orig-Countries_New-ArchFullUrb2v01_prep01_Wt-Pop2010</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14">
+      <c r="B18" t="str">
+        <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
+        <v>STM3_newReceive_Orig-Countries_New-ArchFullUrb2v01_prep01_urb_Wt-Pop2010</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" t="str">
+        <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
+        <v>STM3_newReceive_Orig-Countries_New-ArchFullUrb2v01_prep01_urb_Wt-Pop2010</v>
+      </c>
+      <c r="H18" t="s">
+        <v>194</v>
+      </c>
+      <c r="I18" t="s">
+        <v>116</v>
+      </c>
+      <c r="J18" t="s">
+        <v>28</v>
+      </c>
+      <c r="K18" t="s">
+        <v>274</v>
+      </c>
+      <c r="L18" t="s">
+        <v>32</v>
+      </c>
+      <c r="M18" t="b">
+        <v>1</v>
+      </c>
+      <c r="N18" s="14" t="str">
+        <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_Wt-"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
+        <v>STM3_newReceive_Orig-Countries_New-ArchFullUrb2v01_prep01_urb_Wt-Pop2010</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14">
+      <c r="B19" t="str">
+        <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
+        <v>STM3_newEmit_Orig-Countries_New-ArchFullUrb2v01_prep01_Wt-Pop2010</v>
+      </c>
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" t="str">
+        <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
+        <v>STM3_newEmit_Orig-Countries_New-ArchFullUrb2v01_prep01_Wt-Pop2010</v>
+      </c>
+      <c r="H19" t="s">
+        <v>194</v>
+      </c>
+      <c r="I19" t="s">
+        <v>117</v>
+      </c>
+      <c r="J19" t="s">
+        <v>28</v>
+      </c>
+      <c r="K19" t="s">
+        <v>272</v>
+      </c>
+      <c r="L19" t="s">
+        <v>32</v>
+      </c>
+      <c r="M19" t="b">
+        <v>1</v>
+      </c>
+      <c r="N19" s="14" t="str">
+        <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_Wt-"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
+        <v>STM3_newEmit_Orig-Countries_New-ArchFullUrb2v01_prep01_Wt-Pop2010</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14">
+      <c r="B20" t="str">
+        <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
+        <v>STM3_newEmit_Orig-Countries_New-ArchFullUrb2v01_prep01_urb_Wt-Pop2010</v>
+      </c>
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" t="str">
+        <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
+        <v>STM3_newEmit_Orig-Countries_New-ArchFullUrb2v01_prep01_urb_Wt-Pop2010</v>
+      </c>
+      <c r="H20" t="s">
+        <v>194</v>
+      </c>
+      <c r="I20" t="s">
+        <v>117</v>
+      </c>
+      <c r="J20" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" t="s">
+        <v>274</v>
+      </c>
+      <c r="L20" t="s">
+        <v>32</v>
+      </c>
+      <c r="M20" t="b">
+        <v>1</v>
+      </c>
+      <c r="N20" s="14" t="str">
+        <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_Wt-"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
+        <v>STM3_newEmit_Orig-Countries_New-ArchFullUrb2v01_prep01_urb_Wt-Pop2010</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I11:I14" xr:uid="{E821405C-6957-4A9F-8765-11FEDC830D01}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I11:I20" xr:uid="{E821405C-6957-4A9F-8765-11FEDC830D01}">
       <formula1>list.STM_types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L11:L14" xr:uid="{5BDCD423-46E4-4A7B-8628-5C9344A21620}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L11:L20" xr:uid="{5BDCD423-46E4-4A7B-8628-5C9344A21620}">
       <formula1>list.Data_unique</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M11:M14" xr:uid="{30B9C429-7EFE-4DEB-8979-C009F9C29D27}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M11:M20" xr:uid="{30B9C429-7EFE-4DEB-8979-C009F9C29D27}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J11:K14" xr:uid="{3AF342F9-C154-4566-A6D6-DF321DDA9F17}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J11:K20" xr:uid="{3AF342F9-C154-4566-A6D6-DF321DDA9F17}">
       <formula1>list.Files_geo_unique</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>